<commit_message>
fix: typos on menu
</commit_message>
<xml_diff>
--- a/Excel/Hjemmelaga_sandwich.xlsx
+++ b/Excel/Hjemmelaga_sandwich.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaja_\Dokumenter\Webtek\Excel_to_text\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaja_\Dokumenter\Webtek\Nettside_webtek_28\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E09B7685-5D4C-4CB4-9E57-EB5205ADE339}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6EBE045-EF93-4ECF-A3E6-5D7D0080E3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5424" yWindow="1836" windowWidth="17280" windowHeight="8964" xr2:uid="{55D45A5A-2E26-4BF4-94F2-789971F29FCB}"/>
+    <workbookView xWindow="1248" yWindow="264" windowWidth="16968" windowHeight="11832" xr2:uid="{55D45A5A-2E26-4BF4-94F2-789971F29FCB}"/>
   </bookViews>
   <sheets>
     <sheet name="Hjemmelaga sandwichbrød" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
     <t xml:space="preserve">Sandwich m/ kyllingfilet og bacon </t>
   </si>
   <si>
-    <t>aioli, salat, agurk, paprika, rødløk og tomat. 1,2,3,10,12</t>
+    <t>aioli, salat, agurk, paprika, raudlauk og tomat. 1,2,3,10,12</t>
   </si>
 </sst>
 </file>
@@ -417,7 +417,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>